<commit_message>
fixed arrays and conditions
</commit_message>
<xml_diff>
--- a/temporary/students_table.xlsx
+++ b/temporary/students_table.xlsx
@@ -1505,6 +1505,192 @@
         </is>
       </c>
     </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>Md. Masuk Al Hussain </t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>Tarik Hossain</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>2023-05-28</t>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>Rajshahi</t>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="G25" s="0" t="inlineStr">
+        <is>
+          <t>Islam</t>
+        </is>
+      </c>
+      <c r="H25" s="0" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="I25" s="0" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="J25" s="0" t="inlineStr">
+        <is>
+          <t>A+</t>
+        </is>
+      </c>
+      <c r="K25" s="0" t="inlineStr">
+        <is>
+          <t>masukalhussain3@gmail.com</t>
+        </is>
+      </c>
+      <c r="L25" s="0" t="inlineStr">
+        <is>
+          <t>01709014797</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>Ziyana Islam</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>Quamrul Islam</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>2019-01-10</t>
+        </is>
+      </c>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t>Dhaka, Bangladesh</t>
+        </is>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="G26" s="0" t="inlineStr">
+        <is>
+          <t>Islam</t>
+        </is>
+      </c>
+      <c r="H26" s="0" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="I26" s="0" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="J26" s="0" t="inlineStr">
+        <is>
+          <t>A+</t>
+        </is>
+      </c>
+      <c r="K26" s="0" t="inlineStr">
+        <is>
+          <t>ziyana@gmail.com</t>
+        </is>
+      </c>
+      <c r="L26" s="0" t="inlineStr">
+        <is>
+          <t>01709014797</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>Affan Islam</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>Salman Islam</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>Dhaka, Bangladesh</t>
+        </is>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="G27" s="0" t="inlineStr">
+        <is>
+          <t>Islam</t>
+        </is>
+      </c>
+      <c r="H27" s="0" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="I27" s="0" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="J27" s="0" t="inlineStr">
+        <is>
+          <t>A+</t>
+        </is>
+      </c>
+      <c r="K27" s="0" t="inlineStr">
+        <is>
+          <t>affan@gmail.com</t>
+        </is>
+      </c>
+      <c r="L27" s="0" t="inlineStr">
+        <is>
+          <t>01709014797</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>